<commit_message>
Fixed some benchmark + plot on LaTeX
</commit_message>
<xml_diff>
--- a/BenchCDH(CharmLib).xlsx
+++ b/BenchCDH(CharmLib).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UnInsu\CryptoThesis\Commitment_Schemes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6003457C-058B-45CB-BE75-650BB3EBB77E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D53E613-81D0-4357-90F4-3E20BDB58AF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -389,7 +389,7 @@
   <dimension ref="B1:G34"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -453,7 +453,7 @@
         <v>1.61647796630859E-4</v>
       </c>
       <c r="G3" s="1">
-        <v>1.983642578125E-4</v>
+        <v>3.6144256591796799E-4</v>
       </c>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.25">
@@ -561,7 +561,7 @@
         <v>1.6832351684570299E-4</v>
       </c>
       <c r="G15" s="1">
-        <v>3.3140182495117101E-4</v>
+        <v>2.0140182495117099E-4</v>
       </c>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.25">
@@ -717,7 +717,7 @@
         <v>0.23816847801208399</v>
       </c>
       <c r="E34" s="1">
-        <v>3.3162832260131801E-2</v>
+        <v>3.91628322601318E-2</v>
       </c>
       <c r="F34" s="1">
         <v>4.2510032653808502E-4</v>

</xml_diff>